<commit_message>
Student Presentation Gui Display pending booking presentation - DEVELOP
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
+++ b/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olaf\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olaf\IdeaProjects\OODJ\src\main\resources\Data\SampleDataXlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B70247F9-816F-4773-9D8E-163B12FEA26A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23A7795-F2D0-4A2C-83C0-43D1D5E900F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23145" yWindow="0" windowWidth="15255" windowHeight="21000" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1695" yWindow="1365" windowWidth="18255" windowHeight="17550" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -791,13 +791,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1135,7 +1134,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" t="s">
         <v>86</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -1170,7 +1169,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" t="s">
         <v>181</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -3375,7 +3374,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Student Presentation Gui Display All Details - DEVELOP
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
+++ b/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olaf\IdeaProjects\OODJ\src\main\resources\Data\SampleDataXlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanh\IdeaProjects\G5-2402-OODJ\src\main\resources\Data\SampleDataXlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E23A7795-F2D0-4A2C-83C0-43D1D5E900F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7226A0A9-4891-490A-BCA3-3A391D8FB37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1695" yWindow="1365" windowWidth="18255" windowHeight="17550" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6015" yWindow="2430" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="245">
   <si>
     <t>id</t>
   </si>
@@ -750,6 +750,21 @@
   </si>
   <si>
     <t>2022-04-09 00:00:00</t>
+  </si>
+  <si>
+    <t>PENDING_CONFIRM</t>
+  </si>
+  <si>
+    <t>REJECTED</t>
+  </si>
+  <si>
+    <t>BOOKED</t>
+  </si>
+  <si>
+    <t>MARKED</t>
+  </si>
+  <si>
+    <t>OVERDUE</t>
   </si>
 </sst>
 </file>
@@ -3374,7 +3389,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3541,7 +3556,7 @@
         <v>85</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>159</v>
+        <v>240</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>128</v>
@@ -3637,7 +3652,7 @@
         <v>85</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>159</v>
+        <v>241</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>128</v>
@@ -3733,7 +3748,7 @@
         <v>85</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>159</v>
+        <v>242</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>128</v>
@@ -3829,7 +3844,7 @@
         <v>85</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>159</v>
+        <v>243</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>128</v>
@@ -3925,7 +3940,7 @@
         <v>85</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>159</v>
+        <v>244</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>128</v>

</xml_diff>

<commit_message>
Student Presentation Booking Function - DEVELOP
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
+++ b/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanh\IdeaProjects\G5-2402-OODJ\src\main\resources\Data\SampleDataXlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olaf\IdeaProjects\OODJ\src\main\resources\Data\SampleDataXlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7226A0A9-4891-490A-BCA3-3A391D8FB37E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF064DA-7F86-4257-B78F-4FFD697B8BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6015" yWindow="2430" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1695" yWindow="1365" windowWidth="18255" windowHeight="17550" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="241">
   <si>
     <t>id</t>
   </si>
@@ -383,9 +383,6 @@
     <t>ENVIRONMENT ISSUES IN MALAYSIA</t>
   </si>
   <si>
-    <t>2023-04-09</t>
-  </si>
-  <si>
     <t>firstMarkerId</t>
   </si>
   <si>
@@ -746,25 +743,16 @@
     <t>3268572</t>
   </si>
   <si>
-    <t>2023-04-09 00:00:00</t>
-  </si>
-  <si>
     <t>2022-04-09 00:00:00</t>
   </si>
   <si>
-    <t>PENDING_CONFIRM</t>
-  </si>
-  <si>
-    <t>REJECTED</t>
-  </si>
-  <si>
-    <t>BOOKED</t>
-  </si>
-  <si>
-    <t>MARKED</t>
-  </si>
-  <si>
-    <t>OVERDUE</t>
+    <t>2026-01-01</t>
+  </si>
+  <si>
+    <t>2024-08-01</t>
+  </si>
+  <si>
+    <t>2024-08-01 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -1185,7 +1173,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
@@ -1220,7 +1208,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -1255,7 +1243,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
@@ -1290,7 +1278,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -1325,7 +1313,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -1360,7 +1348,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
@@ -1395,7 +1383,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>23</v>
@@ -1430,7 +1418,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>25</v>
@@ -1465,7 +1453,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>41</v>
@@ -1500,7 +1488,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>43</v>
@@ -1535,7 +1523,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>45</v>
@@ -1570,7 +1558,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>46</v>
@@ -1605,7 +1593,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>47</v>
@@ -1640,7 +1628,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>44</v>
@@ -1675,7 +1663,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>48</v>
@@ -1716,7 +1704,7 @@
         <v>60</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>59</v>
@@ -1755,7 +1743,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="D2" sqref="D2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1793,7 +1781,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>91</v>
@@ -1802,10 +1790,10 @@
         <v>92</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>97</v>
+        <v>238</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>100</v>
@@ -1816,7 +1804,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>93</v>
@@ -1842,6 +1830,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1849,8 +1838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9D51FCF-93DA-4829-9D15-DA3415652AC5}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1879,7 +1868,7 @@
         <v>102</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>103</v>
@@ -1899,28 +1888,28 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>106</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>85</v>
@@ -1934,25 +1923,25 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>107</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>85</v>
@@ -1963,28 +1952,28 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>108</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>85</v>
@@ -1995,28 +1984,28 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>109</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>85</v>
@@ -2027,28 +2016,28 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>110</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>85</v>
@@ -2059,28 +2048,28 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>111</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>85</v>
@@ -2091,28 +2080,28 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>112</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>96</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>100</v>
@@ -2123,28 +2112,28 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>96</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>100</v>
@@ -2155,28 +2144,28 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>96</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>100</v>
@@ -2187,28 +2176,28 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>115</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>96</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>100</v>
@@ -2219,28 +2208,28 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>116</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>96</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>100</v>
@@ -2260,8 +2249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBCA89A-312D-41B5-8992-19B0B67944A1}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2282,31 +2271,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>4</v>
@@ -2317,28 +2306,28 @@
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="H2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>85</v>
@@ -2355,28 +2344,28 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>85</v>
@@ -2393,28 +2382,28 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>85</v>
@@ -2431,28 +2420,28 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>101</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>85</v>
@@ -2469,28 +2458,28 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>101</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>85</v>
@@ -2507,28 +2496,28 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>101</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>85</v>
@@ -2545,28 +2534,28 @@
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>85</v>
@@ -2583,28 +2572,28 @@
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="H9" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>85</v>
@@ -2621,28 +2610,28 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>85</v>
@@ -2659,28 +2648,28 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>85</v>
@@ -2697,28 +2686,28 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>85</v>
@@ -2735,28 +2724,28 @@
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>85</v>
@@ -2773,28 +2762,28 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F14" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="H14" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>85</v>
@@ -2811,28 +2800,28 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="H15" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>85</v>
@@ -2849,28 +2838,28 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>177</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>85</v>
@@ -2887,28 +2876,28 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>85</v>
@@ -2925,28 +2914,28 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>85</v>
@@ -2963,28 +2952,28 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>117</v>
+        <v>239</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>85</v>
@@ -3001,28 +2990,28 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>100</v>
@@ -3039,28 +3028,28 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>100</v>
@@ -3077,28 +3066,28 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>100</v>
@@ -3115,28 +3104,28 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>100</v>
@@ -3153,28 +3142,28 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>100</v>
@@ -3191,28 +3180,28 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>100</v>
@@ -3229,28 +3218,28 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>100</v>
@@ -3267,28 +3256,28 @@
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>100</v>
@@ -3305,28 +3294,28 @@
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>100</v>
@@ -3343,28 +3332,28 @@
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>100</v>
@@ -3381,6 +3370,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3389,7 +3379,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3413,25 +3403,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>4</v>
@@ -3442,28 +3432,28 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>85</v>
@@ -3474,28 +3464,28 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>85</v>
@@ -3506,28 +3496,28 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>85</v>
@@ -3538,28 +3528,28 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>101</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>240</v>
+        <v>158</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>85</v>
@@ -3570,28 +3560,28 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>101</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>85</v>
@@ -3602,28 +3592,28 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>85</v>
@@ -3634,28 +3624,28 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>241</v>
+        <v>158</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>85</v>
@@ -3666,28 +3656,28 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>85</v>
@@ -3698,28 +3688,28 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>85</v>
@@ -3730,28 +3720,28 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>242</v>
+        <v>158</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>85</v>
@@ -3762,28 +3752,28 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>85</v>
@@ -3794,28 +3784,28 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>85</v>
@@ -3826,28 +3816,28 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>191</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>243</v>
+        <v>158</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>85</v>
@@ -3858,28 +3848,28 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>85</v>
@@ -3890,28 +3880,28 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>85</v>
@@ -3922,28 +3912,28 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>244</v>
+        <v>158</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>85</v>
@@ -3954,28 +3944,28 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>85</v>
@@ -3986,28 +3976,28 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>85</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>100</v>
@@ -4018,28 +4008,28 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>100</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>100</v>
@@ -4050,28 +4040,28 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>100</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>100</v>
@@ -4082,28 +4072,28 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>100</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>100</v>
@@ -4114,28 +4104,28 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>100</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>100</v>
@@ -4146,28 +4136,28 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>100</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>100</v>
@@ -4178,28 +4168,28 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>100</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>100</v>
@@ -4210,28 +4200,28 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>100</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>100</v>
@@ -4242,28 +4232,28 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>100</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>100</v>
@@ -4274,28 +4264,28 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>100</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>100</v>
@@ -4306,28 +4296,28 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>100</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>100</v>
@@ -4339,6 +4329,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4366,16 +4357,16 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
@@ -4386,163 +4377,163 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="F6" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>129</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Presentation Edit, Re-schedule, View Result Function - DEVELOP
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
+++ b/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olaf\IdeaProjects\OODJ\src\main\resources\Data\SampleDataXlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanh\IdeaProjects\G5-2402-OODJ\src\main\resources\Data\SampleDataXlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DF064DA-7F86-4257-B78F-4FFD697B8BA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353C9D5A-90A3-492B-ADE8-CD85D359A655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1695" yWindow="1365" windowWidth="18255" windowHeight="17550" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="242">
   <si>
     <t>id</t>
   </si>
@@ -752,7 +752,10 @@
     <t>2024-08-01</t>
   </si>
   <si>
-    <t>2024-08-01 00:00:00</t>
+    <t>2024-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>2024-04-09 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -1839,7 +1842,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H7"/>
+      <selection activeCell="G2" sqref="G2:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3379,7 +3382,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="H3" sqref="H3:H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3444,10 +3447,10 @@
         <v>190</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>85</v>
+        <v>240</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>158</v>
@@ -3476,10 +3479,10 @@
         <v>191</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>85</v>
+        <v>240</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>158</v>
@@ -3508,10 +3511,10 @@
         <v>192</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>85</v>
+        <v>240</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>158</v>
@@ -3540,10 +3543,10 @@
         <v>190</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>85</v>
+        <v>240</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>158</v>
@@ -3572,10 +3575,10 @@
         <v>191</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>85</v>
+        <v>240</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>158</v>
@@ -3604,10 +3607,10 @@
         <v>192</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>85</v>
+        <v>240</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>158</v>
@@ -3636,10 +3639,10 @@
         <v>190</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>85</v>
+        <v>240</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>158</v>
@@ -3668,10 +3671,10 @@
         <v>191</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>158</v>
@@ -3700,10 +3703,10 @@
         <v>192</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>158</v>
@@ -3732,10 +3735,10 @@
         <v>190</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>158</v>
@@ -3764,10 +3767,10 @@
         <v>191</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>158</v>
@@ -3796,10 +3799,10 @@
         <v>192</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>158</v>
@@ -3828,10 +3831,10 @@
         <v>190</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>158</v>
@@ -3860,10 +3863,10 @@
         <v>191</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>158</v>
@@ -3892,10 +3895,10 @@
         <v>192</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>158</v>
@@ -3924,10 +3927,10 @@
         <v>190</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>158</v>
@@ -3956,10 +3959,10 @@
         <v>191</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>158</v>
@@ -3988,10 +3991,10 @@
         <v>192</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>85</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>158</v>

</xml_diff>

<commit_message>
Submission Object Class remove parameter - UPDATE
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
+++ b/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanh\IdeaProjects\G5-2402-OODJ\src\main\resources\Data\SampleDataXlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353C9D5A-90A3-492B-ADE8-CD85D359A655}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E059E015-1260-4150-990F-E96C65F42149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4410" yWindow="3060" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="274">
   <si>
     <t>id</t>
   </si>
@@ -752,10 +752,106 @@
     <t>2024-08-01</t>
   </si>
   <si>
+    <t>PENDING_CONFIRM</t>
+  </si>
+  <si>
     <t>2024-01-01 00:00:00</t>
   </si>
   <si>
-    <t>2024-04-09 00:00:00</t>
+    <t>REJECTED</t>
+  </si>
+  <si>
+    <t>MARKED</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>BOOKED</t>
+  </si>
+  <si>
+    <t>OVERDUE</t>
+  </si>
+  <si>
+    <t>2024-08-01 00:00:00</t>
   </si>
 </sst>
 </file>
@@ -1746,7 +1842,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:E2"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,7 +1938,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H12"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2252,8 +2348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBCA89A-312D-41B5-8992-19B0B67944A1}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3381,8 +3477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E9194B5-C6E7-4E5D-9E57-7889554C77E2}">
   <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3:H29"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3447,16 +3543,16 @@
         <v>190</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>127</v>
+        <v>244</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>85</v>
@@ -3479,16 +3575,16 @@
         <v>191</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>127</v>
+        <v>245</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>85</v>
@@ -3511,16 +3607,16 @@
         <v>192</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>127</v>
+        <v>246</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>85</v>
@@ -3543,16 +3639,16 @@
         <v>190</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="H5" s="1" t="s">
-        <v>127</v>
+        <v>247</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>85</v>
@@ -3575,16 +3671,16 @@
         <v>191</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>127</v>
+        <v>248</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>85</v>
@@ -3607,16 +3703,16 @@
         <v>192</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>127</v>
+        <v>249</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>85</v>
@@ -3639,16 +3735,16 @@
         <v>190</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="G8" s="1" t="s">
-        <v>158</v>
+        <v>242</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>127</v>
+        <v>250</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>85</v>
@@ -3671,16 +3767,16 @@
         <v>191</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>127</v>
+        <v>251</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>85</v>
@@ -3703,16 +3799,16 @@
         <v>192</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>127</v>
+        <v>252</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>85</v>
@@ -3735,16 +3831,16 @@
         <v>190</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="G11" s="1" t="s">
-        <v>158</v>
+        <v>271</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>127</v>
+        <v>253</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>85</v>
@@ -3767,16 +3863,16 @@
         <v>191</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>127</v>
+        <v>254</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>85</v>
@@ -3799,16 +3895,16 @@
         <v>192</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>85</v>
@@ -3831,16 +3927,16 @@
         <v>190</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F14" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="G14" s="1" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>127</v>
+        <v>256</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>85</v>
@@ -3863,16 +3959,16 @@
         <v>191</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>127</v>
+        <v>257</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>85</v>
@@ -3895,16 +3991,16 @@
         <v>192</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F16" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>127</v>
+        <v>258</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>85</v>
@@ -3927,16 +4023,16 @@
         <v>190</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>240</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>158</v>
+        <v>272</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>127</v>
+        <v>259</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>85</v>
@@ -3959,16 +4055,16 @@
         <v>191</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>127</v>
+        <v>260</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>85</v>
@@ -3991,16 +4087,16 @@
         <v>192</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="F19" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>240</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>127</v>
+        <v>261</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>100</v>
@@ -4032,7 +4128,7 @@
         <v>158</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>127</v>
+        <v>262</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>100</v>
@@ -4064,7 +4160,7 @@
         <v>158</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>127</v>
+        <v>263</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>100</v>
@@ -4096,7 +4192,7 @@
         <v>158</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>127</v>
+        <v>244</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>100</v>
@@ -4128,7 +4224,7 @@
         <v>158</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>127</v>
+        <v>264</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>100</v>
@@ -4160,7 +4256,7 @@
         <v>158</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>127</v>
+        <v>265</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>100</v>
@@ -4189,10 +4285,10 @@
         <v>100</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>127</v>
+        <v>266</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>100</v>
@@ -4221,10 +4317,10 @@
         <v>100</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>127</v>
+        <v>267</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>100</v>
@@ -4253,10 +4349,10 @@
         <v>100</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>127</v>
+        <v>268</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>100</v>
@@ -4285,10 +4381,10 @@
         <v>100</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>127</v>
+        <v>269</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>100</v>
@@ -4317,10 +4413,10 @@
         <v>100</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>158</v>
+        <v>243</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>127</v>
+        <v>270</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>100</v>

</xml_diff>

<commit_message>
SubmissionDAO read data into ram - DEVELOP
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
+++ b/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanh\IdeaProjects\G5-2402-OODJ\src\main\resources\Data\SampleDataXlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E059E015-1260-4150-990F-E96C65F42149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE1748C-87DD-4C9C-9654-D7546365C7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4410" yWindow="3060" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -1937,8 +1937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9D51FCF-93DA-4829-9D15-DA3415652AC5}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2349,7 +2349,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2417,7 +2417,7 @@
         <v>190</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>175</v>
@@ -2455,7 +2455,7 @@
         <v>191</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>175</v>
@@ -2493,7 +2493,7 @@
         <v>192</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>175</v>
@@ -2531,7 +2531,7 @@
         <v>190</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>175</v>
@@ -2569,7 +2569,7 @@
         <v>191</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>175</v>
@@ -2607,7 +2607,7 @@
         <v>192</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>175</v>
@@ -2645,7 +2645,7 @@
         <v>190</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>175</v>
@@ -2683,7 +2683,7 @@
         <v>191</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>175</v>
@@ -2721,7 +2721,7 @@
         <v>192</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>175</v>
@@ -2759,7 +2759,7 @@
         <v>190</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>175</v>
@@ -2797,7 +2797,7 @@
         <v>191</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>175</v>
@@ -2835,7 +2835,7 @@
         <v>192</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>175</v>
@@ -2873,7 +2873,7 @@
         <v>190</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>175</v>
@@ -2911,7 +2911,7 @@
         <v>191</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>175</v>
@@ -2949,7 +2949,7 @@
         <v>192</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>175</v>
@@ -2987,7 +2987,7 @@
         <v>190</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>175</v>
@@ -3025,7 +3025,7 @@
         <v>191</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>175</v>
@@ -3063,7 +3063,7 @@
         <v>192</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>175</v>
@@ -3101,7 +3101,7 @@
         <v>193</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>167</v>
+        <v>237</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>175</v>
@@ -3139,7 +3139,7 @@
         <v>94</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>167</v>
+        <v>237</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>175</v>
@@ -3177,7 +3177,7 @@
         <v>193</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>167</v>
+        <v>237</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>175</v>
@@ -3215,7 +3215,7 @@
         <v>94</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>167</v>
+        <v>237</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>175</v>
@@ -3253,7 +3253,7 @@
         <v>193</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>167</v>
+        <v>237</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>175</v>
@@ -3291,7 +3291,7 @@
         <v>94</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>167</v>
+        <v>237</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>175</v>
@@ -3329,7 +3329,7 @@
         <v>193</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>167</v>
+        <v>237</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>175</v>
@@ -3367,7 +3367,7 @@
         <v>94</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>167</v>
+        <v>237</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>175</v>
@@ -3405,7 +3405,7 @@
         <v>193</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>167</v>
+        <v>237</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>175</v>
@@ -3443,7 +3443,7 @@
         <v>94</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>167</v>
+        <v>237</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>175</v>

</xml_diff>

<commit_message>
StudentGui Project Dashboard Display All Information - DEVELOP T^T Inheritance very hard...... SOS
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
+++ b/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanh\IdeaProjects\G5-2402-OODJ\src\main\resources\Data\SampleDataXlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olaf\IdeaProjects\OODJ\src\main\resources\Data\SampleDataXlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BE1748C-87DD-4C9C-9654-D7546365C7C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AAB1EF-BF3F-455F-9141-02E373690588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12390" yWindow="2805" windowWidth="22095" windowHeight="17550" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Submission" sheetId="6" r:id="rId4"/>
     <sheet name="Presentation" sheetId="8" r:id="rId5"/>
     <sheet name="Consultation" sheetId="5" r:id="rId6"/>
+    <sheet name="Report" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="295">
   <si>
     <t>id</t>
   </si>
@@ -852,6 +853,69 @@
   </si>
   <si>
     <t>2024-08-01 00:00:00</t>
+  </si>
+  <si>
+    <t>PENDING_MARKING</t>
+  </si>
+  <si>
+    <t>MARKED_2</t>
+  </si>
+  <si>
+    <t>MARKED_1</t>
+  </si>
+  <si>
+    <t>reportName</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>InvestigateReport</t>
+  </si>
+  <si>
+    <t>FinalYearProject</t>
+  </si>
+  <si>
+    <t>Capstone1</t>
+  </si>
+  <si>
+    <t>Capstone2</t>
+  </si>
+  <si>
+    <t>49053257</t>
+  </si>
+  <si>
+    <t>26662640</t>
+  </si>
+  <si>
+    <t>34685929</t>
+  </si>
+  <si>
+    <t>18449474</t>
+  </si>
+  <si>
+    <t>63860114</t>
+  </si>
+  <si>
+    <t>reportPath</t>
+  </si>
+  <si>
+    <t>src/main/resources/Data/SampleDataXlsx/Report.pdf</t>
+  </si>
+  <si>
+    <t>src/main/resources/Data/SampleDataXlsx/InvestigateReport.pdf</t>
+  </si>
+  <si>
+    <t>src/main/resources/Data/SampleDataXlsx/FinalYearProject.pdf</t>
+  </si>
+  <si>
+    <t>src/main/resources/Data/SampleDataXlsx/Capstone1.pdf</t>
+  </si>
+  <si>
+    <t>src/main/resources/Data/SampleDataXlsx/Capstone2.pdf</t>
+  </si>
+  <si>
+    <t>REPORT</t>
   </si>
 </sst>
 </file>
@@ -2348,8 +2412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBCA89A-312D-41B5-8992-19B0B67944A1}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2534,7 +2598,7 @@
         <v>273</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>175</v>
+        <v>274</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>177</v>
@@ -2648,7 +2712,7 @@
         <v>273</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>175</v>
+        <v>276</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>176</v>
@@ -2762,7 +2826,7 @@
         <v>273</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>175</v>
+        <v>275</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>177</v>
@@ -2876,7 +2940,7 @@
         <v>273</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>175</v>
+        <v>272</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>176</v>
@@ -4437,7 +4501,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4639,4 +4703,109 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C6E3A0-FE14-4583-BA4F-E8188E3B166D}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>277</v>
+      </c>
+      <c r="C1" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2" t="s">
+        <v>278</v>
+      </c>
+      <c r="C2" t="s">
+        <v>289</v>
+      </c>
+      <c r="D2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="B3" t="s">
+        <v>279</v>
+      </c>
+      <c r="C3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>285</v>
+      </c>
+      <c r="B4" t="s">
+        <v>280</v>
+      </c>
+      <c r="C4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B5" t="s">
+        <v>281</v>
+      </c>
+      <c r="C5" t="s">
+        <v>292</v>
+      </c>
+      <c r="D5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="B6" t="s">
+        <v>282</v>
+      </c>
+      <c r="C6" t="s">
+        <v>293</v>
+      </c>
+      <c r="D6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Report Class Create n ReportDAO develop n UUIDHandler develop - DEVELOP
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
+++ b/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olaf\IdeaProjects\OODJ\src\main\resources\Data\SampleDataXlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanh\IdeaProjects\G5-2402-OODJ\src\main\resources\Data\SampleDataXlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71AAB1EF-BF3F-455F-9141-02E373690588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9521175-FBB7-4018-8783-C874790FD460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12390" yWindow="2805" windowWidth="22095" windowHeight="17550" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -1905,8 +1905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ECA981E-FBC4-4953-91F1-E2A23A38E898}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="A4:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4709,7 +4709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C6E3A0-FE14-4583-BA4F-E8188E3B166D}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Student Submit Project Function TODO: Save to txt file - DEVELOP
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
+++ b/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanh\IdeaProjects\G5-2402-OODJ\src\main\resources\Data\SampleDataXlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olaf\IdeaProjects\OODJ\src\main\resources\Data\SampleDataXlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9521175-FBB7-4018-8783-C874790FD460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B72A75-B77B-4B7F-8E47-77A885DFC11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="293">
   <si>
     <t>id</t>
   </si>
@@ -861,9 +861,6 @@
     <t>MARKED_2</t>
   </si>
   <si>
-    <t>MARKED_1</t>
-  </si>
-  <si>
     <t>reportName</t>
   </si>
   <si>
@@ -913,9 +910,6 @@
   </si>
   <si>
     <t>src/main/resources/Data/SampleDataXlsx/Capstone2.pdf</t>
-  </si>
-  <si>
-    <t>REPORT</t>
   </si>
 </sst>
 </file>
@@ -1905,8 +1899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ECA981E-FBC4-4953-91F1-E2A23A38E898}">
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="A4:G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2002,7 +1996,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2413,7 +2407,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2472,7 +2466,7 @@
         <v>207</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>127</v>
+        <v>282</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>197</v>
@@ -2484,7 +2478,7 @@
         <v>273</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>175</v>
+        <v>274</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>176</v>
@@ -2586,7 +2580,7 @@
         <v>210</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>127</v>
+        <v>283</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>101</v>
@@ -2700,7 +2694,7 @@
         <v>213</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>127</v>
+        <v>284</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>198</v>
@@ -2712,7 +2706,7 @@
         <v>273</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>176</v>
@@ -4709,8 +4703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C6E3A0-FE14-4583-BA4F-E8188E3B166D}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4726,10 +4720,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D1" t="s">
         <v>171</v>
@@ -4737,55 +4731,55 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C2" t="s">
-        <v>289</v>
-      </c>
-      <c r="D2" t="s">
-        <v>294</v>
+        <v>288</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C3" t="s">
-        <v>290</v>
-      </c>
-      <c r="D3" t="s">
-        <v>176</v>
+        <v>289</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B4" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C4" t="s">
-        <v>291</v>
-      </c>
-      <c r="D4" t="s">
-        <v>177</v>
+        <v>290</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B5" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D5" t="s">
         <v>178</v>
@@ -4793,13 +4787,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B6" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C6" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D6" t="s">
         <v>179</v>
@@ -4807,5 +4801,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Student Remove Submission Function - DEVELOP
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
+++ b/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olaf\IdeaProjects\OODJ\src\main\resources\Data\SampleDataXlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanh\IdeaProjects\G5-2402-OODJ\src\main\resources\Data\SampleDataXlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B72A75-B77B-4B7F-8E47-77A885DFC11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D024291B-B407-42FD-BC6B-2353E1CAED79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -858,9 +858,6 @@
     <t>PENDING_MARKING</t>
   </si>
   <si>
-    <t>MARKED_2</t>
-  </si>
-  <si>
     <t>reportName</t>
   </si>
   <si>
@@ -910,6 +907,9 @@
   </si>
   <si>
     <t>src/main/resources/Data/SampleDataXlsx/Capstone2.pdf</t>
+  </si>
+  <si>
+    <t>REPORT</t>
   </si>
 </sst>
 </file>
@@ -1900,7 +1900,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2406,8 +2406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBCA89A-312D-41B5-8992-19B0B67944A1}">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2466,7 +2466,7 @@
         <v>207</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>197</v>
@@ -2481,7 +2481,7 @@
         <v>274</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>176</v>
+        <v>292</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>127</v>
@@ -2580,7 +2580,7 @@
         <v>210</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>101</v>
@@ -2694,7 +2694,7 @@
         <v>213</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>198</v>
@@ -2808,7 +2808,7 @@
         <v>216</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>127</v>
+        <v>284</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>199</v>
@@ -2820,10 +2820,10 @@
         <v>273</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>127</v>
@@ -2922,7 +2922,7 @@
         <v>219</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>127</v>
+        <v>285</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>200</v>
@@ -2934,10 +2934,10 @@
         <v>273</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>127</v>
@@ -4494,9 +4494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1196795C-F429-445C-983E-375FDEA16CC7}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4703,8 +4701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C6E3A0-FE14-4583-BA4F-E8188E3B166D}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4720,10 +4718,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D1" t="s">
         <v>171</v>
@@ -4731,21 +4729,21 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>176</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B3" t="s">
         <v>278</v>
@@ -4759,13 +4757,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>176</v>
@@ -4773,13 +4771,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B5" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D5" t="s">
         <v>178</v>
@@ -4787,13 +4785,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B6" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C6" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D6" t="s">
         <v>179</v>

</xml_diff>

<commit_message>
Student Display Report Result (TODO Add Comment Parameter) - DEVELOP
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
+++ b/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanh\IdeaProjects\G5-2402-OODJ\src\main\resources\Data\SampleDataXlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D024291B-B407-42FD-BC6B-2353E1CAED79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3B9D12-0821-4DD8-BC9C-0CA4D2DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6615" yWindow="30" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -855,9 +855,6 @@
     <t>2024-08-01 00:00:00</t>
   </si>
   <si>
-    <t>PENDING_MARKING</t>
-  </si>
-  <si>
     <t>reportName</t>
   </si>
   <si>
@@ -910,6 +907,9 @@
   </si>
   <si>
     <t>REPORT</t>
+  </si>
+  <si>
+    <t>MARKED_2</t>
   </si>
 </sst>
 </file>
@@ -2407,7 +2407,7 @@
   <dimension ref="A1:L29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2466,7 +2466,7 @@
         <v>207</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>197</v>
@@ -2478,13 +2478,13 @@
         <v>273</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>274</v>
+        <v>292</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>85</v>
@@ -2516,13 +2516,13 @@
         <v>273</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>175</v>
+        <v>292</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>176</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>85</v>
@@ -2554,13 +2554,13 @@
         <v>273</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>175</v>
+        <v>292</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>176</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>85</v>
@@ -2580,7 +2580,7 @@
         <v>210</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>101</v>
@@ -2592,13 +2592,13 @@
         <v>273</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>274</v>
+        <v>292</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>177</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>85</v>
@@ -2630,13 +2630,13 @@
         <v>273</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>175</v>
+        <v>292</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>177</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>85</v>
@@ -2668,13 +2668,13 @@
         <v>273</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>175</v>
+        <v>292</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>177</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>85</v>
@@ -2694,7 +2694,7 @@
         <v>213</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>198</v>
@@ -2706,13 +2706,13 @@
         <v>273</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>274</v>
+        <v>292</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>176</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>85</v>
@@ -2744,13 +2744,13 @@
         <v>273</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>175</v>
+        <v>292</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>176</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>85</v>
@@ -2782,13 +2782,13 @@
         <v>273</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>175</v>
+        <v>292</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>176</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>85</v>
@@ -2808,7 +2808,7 @@
         <v>216</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>199</v>
@@ -2820,13 +2820,13 @@
         <v>273</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>274</v>
+        <v>292</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>178</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>85</v>
@@ -2858,13 +2858,13 @@
         <v>273</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>175</v>
+        <v>292</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>177</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>85</v>
@@ -2896,13 +2896,13 @@
         <v>273</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>175</v>
+        <v>292</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>177</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>85</v>
@@ -2922,7 +2922,7 @@
         <v>219</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>200</v>
@@ -2934,13 +2934,13 @@
         <v>273</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>274</v>
+        <v>292</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>179</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>85</v>
@@ -2972,13 +2972,13 @@
         <v>273</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>175</v>
+        <v>292</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>176</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>85</v>
@@ -3010,13 +3010,13 @@
         <v>273</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>175</v>
+        <v>292</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>176</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>127</v>
+        <v>255</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>85</v>
@@ -3048,7 +3048,7 @@
         <v>273</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>175</v>
+        <v>292</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>177</v>
@@ -4718,10 +4718,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D1" t="s">
         <v>171</v>
@@ -4729,27 +4729,27 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="C3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>177</v>
@@ -4757,13 +4757,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>176</v>
@@ -4771,13 +4771,13 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="C5" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D5" t="s">
         <v>178</v>
@@ -4785,13 +4785,13 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B6" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C6" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D6" t="s">
         <v>179</v>

</xml_diff>

<commit_message>
Student Project Delete Function Bug Fix - UPDATE
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
+++ b/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanh\IdeaProjects\G5-2402-OODJ\src\main\resources\Data\SampleDataXlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olaf\IdeaProjects\OODJ\src\main\resources\Data\SampleDataXlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3B9D12-0821-4DD8-BC9C-0CA4D2DCA74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02382B9-25BC-4408-A4EA-F56178C959DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6615" yWindow="30" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11730" yWindow="2715" windowWidth="22095" windowHeight="17550" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1057" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="306">
   <si>
     <t>id</t>
   </si>
@@ -858,58 +858,97 @@
     <t>reportName</t>
   </si>
   <si>
-    <t>Report</t>
-  </si>
-  <si>
-    <t>InvestigateReport</t>
-  </si>
-  <si>
-    <t>FinalYearProject</t>
-  </si>
-  <si>
-    <t>Capstone1</t>
-  </si>
-  <si>
-    <t>Capstone2</t>
-  </si>
-  <si>
-    <t>49053257</t>
-  </si>
-  <si>
-    <t>26662640</t>
-  </si>
-  <si>
-    <t>34685929</t>
-  </si>
-  <si>
-    <t>18449474</t>
-  </si>
-  <si>
-    <t>63860114</t>
-  </si>
-  <si>
     <t>reportPath</t>
   </si>
   <si>
-    <t>src/main/resources/Data/SampleDataXlsx/Report.pdf</t>
-  </si>
-  <si>
-    <t>src/main/resources/Data/SampleDataXlsx/InvestigateReport.pdf</t>
-  </si>
-  <si>
-    <t>src/main/resources/Data/SampleDataXlsx/FinalYearProject.pdf</t>
-  </si>
-  <si>
-    <t>src/main/resources/Data/SampleDataXlsx/Capstone1.pdf</t>
-  </si>
-  <si>
-    <t>src/main/resources/Data/SampleDataXlsx/Capstone2.pdf</t>
-  </si>
-  <si>
     <t>REPORT</t>
   </si>
   <si>
-    <t>MARKED_2</t>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>comment1</t>
+  </si>
+  <si>
+    <t>comment2</t>
+  </si>
+  <si>
+    <t>comment3</t>
+  </si>
+  <si>
+    <t>comment4</t>
+  </si>
+  <si>
+    <t>comment5</t>
+  </si>
+  <si>
+    <t>comment6</t>
+  </si>
+  <si>
+    <t>comment7</t>
+  </si>
+  <si>
+    <t>comment8</t>
+  </si>
+  <si>
+    <t>comment9</t>
+  </si>
+  <si>
+    <t>comment10</t>
+  </si>
+  <si>
+    <t>comment11</t>
+  </si>
+  <si>
+    <t>comment12</t>
+  </si>
+  <si>
+    <t>comment13</t>
+  </si>
+  <si>
+    <t>comment14</t>
+  </si>
+  <si>
+    <t>comment15</t>
+  </si>
+  <si>
+    <t>comment16</t>
+  </si>
+  <si>
+    <t>comment17</t>
+  </si>
+  <si>
+    <t>comment18</t>
+  </si>
+  <si>
+    <t>comment19</t>
+  </si>
+  <si>
+    <t>comment20</t>
+  </si>
+  <si>
+    <t>comment21</t>
+  </si>
+  <si>
+    <t>comment22</t>
+  </si>
+  <si>
+    <t>comment23</t>
+  </si>
+  <si>
+    <t>comment24</t>
+  </si>
+  <si>
+    <t>comment25</t>
+  </si>
+  <si>
+    <t>comment26</t>
+  </si>
+  <si>
+    <t>comment27</t>
+  </si>
+  <si>
+    <t>comment28</t>
   </si>
 </sst>
 </file>
@@ -2404,10 +2443,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBCA89A-312D-41B5-8992-19B0B67944A1}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2418,12 +2457,12 @@
     <col min="5" max="5" width="19" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="8" max="9" width="12.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="13" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2449,24 +2488,27 @@
         <v>172</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>207</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>280</v>
+        <v>127</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>197</v>
@@ -2478,16 +2520,16 @@
         <v>273</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>292</v>
+        <v>272</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>255</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>85</v>
+        <v>278</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>85</v>
@@ -2498,8 +2540,11 @@
       <c r="L2" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>208</v>
       </c>
@@ -2516,7 +2561,7 @@
         <v>273</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>292</v>
+        <v>175</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>176</v>
@@ -2525,7 +2570,7 @@
         <v>255</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>85</v>
+        <v>279</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>85</v>
@@ -2536,8 +2581,11 @@
       <c r="L3" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>209</v>
       </c>
@@ -2554,7 +2602,7 @@
         <v>273</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>292</v>
+        <v>175</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>176</v>
@@ -2563,7 +2611,7 @@
         <v>255</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>85</v>
+        <v>280</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>85</v>
@@ -2574,13 +2622,16 @@
       <c r="L4" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>210</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>281</v>
+        <v>127</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>101</v>
@@ -2592,7 +2643,7 @@
         <v>273</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>292</v>
+        <v>175</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>177</v>
@@ -2601,7 +2652,7 @@
         <v>255</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>85</v>
+        <v>281</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>85</v>
@@ -2612,8 +2663,11 @@
       <c r="L5" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>211</v>
       </c>
@@ -2630,7 +2684,7 @@
         <v>273</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>292</v>
+        <v>175</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>177</v>
@@ -2639,7 +2693,7 @@
         <v>255</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>85</v>
+        <v>282</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>85</v>
@@ -2650,8 +2704,11 @@
       <c r="L6" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>212</v>
       </c>
@@ -2668,7 +2725,7 @@
         <v>273</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>292</v>
+        <v>175</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>177</v>
@@ -2677,7 +2734,7 @@
         <v>255</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>85</v>
+        <v>283</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>85</v>
@@ -2688,13 +2745,16 @@
       <c r="L7" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>213</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>282</v>
+        <v>127</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>198</v>
@@ -2706,7 +2766,7 @@
         <v>273</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>292</v>
+        <v>175</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>176</v>
@@ -2715,7 +2775,7 @@
         <v>255</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>85</v>
+        <v>284</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>85</v>
@@ -2726,8 +2786,11 @@
       <c r="L8" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>214</v>
       </c>
@@ -2744,7 +2807,7 @@
         <v>273</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>292</v>
+        <v>175</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>176</v>
@@ -2753,7 +2816,7 @@
         <v>255</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>85</v>
+        <v>285</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>85</v>
@@ -2764,8 +2827,11 @@
       <c r="L9" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>215</v>
       </c>
@@ -2782,7 +2848,7 @@
         <v>273</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>292</v>
+        <v>175</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>176</v>
@@ -2791,7 +2857,7 @@
         <v>255</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>85</v>
+        <v>286</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>85</v>
@@ -2802,13 +2868,16 @@
       <c r="L10" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>216</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>283</v>
+        <v>127</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>199</v>
@@ -2820,7 +2889,7 @@
         <v>273</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>292</v>
+        <v>175</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>178</v>
@@ -2829,7 +2898,7 @@
         <v>255</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>85</v>
+        <v>287</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>85</v>
@@ -2840,8 +2909,11 @@
       <c r="L11" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>217</v>
       </c>
@@ -2858,7 +2930,7 @@
         <v>273</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>292</v>
+        <v>175</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>177</v>
@@ -2867,7 +2939,7 @@
         <v>255</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>85</v>
+        <v>288</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>85</v>
@@ -2878,8 +2950,11 @@
       <c r="L12" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>218</v>
       </c>
@@ -2896,7 +2971,7 @@
         <v>273</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>292</v>
+        <v>175</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>177</v>
@@ -2905,7 +2980,7 @@
         <v>255</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>85</v>
+        <v>289</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>85</v>
@@ -2916,13 +2991,16 @@
       <c r="L13" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>219</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>284</v>
+        <v>127</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>200</v>
@@ -2934,7 +3012,7 @@
         <v>273</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>292</v>
+        <v>175</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>179</v>
@@ -2943,7 +3021,7 @@
         <v>255</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>85</v>
+        <v>290</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>85</v>
@@ -2954,8 +3032,11 @@
       <c r="L14" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>220</v>
       </c>
@@ -2972,7 +3053,7 @@
         <v>273</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>292</v>
+        <v>175</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>176</v>
@@ -2981,7 +3062,7 @@
         <v>255</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>85</v>
+        <v>291</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>85</v>
@@ -2992,8 +3073,11 @@
       <c r="L15" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>221</v>
       </c>
@@ -3010,7 +3094,7 @@
         <v>273</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>292</v>
+        <v>175</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>176</v>
@@ -3019,7 +3103,7 @@
         <v>255</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>85</v>
+        <v>292</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>85</v>
@@ -3030,8 +3114,11 @@
       <c r="L16" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>222</v>
       </c>
@@ -3048,7 +3135,7 @@
         <v>273</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>292</v>
+        <v>175</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>177</v>
@@ -3057,7 +3144,7 @@
         <v>127</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>85</v>
+        <v>293</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>85</v>
@@ -3068,8 +3155,11 @@
       <c r="L17" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>223</v>
       </c>
@@ -3095,7 +3185,7 @@
         <v>127</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>85</v>
+        <v>294</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>85</v>
@@ -3106,8 +3196,11 @@
       <c r="L18" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>224</v>
       </c>
@@ -3133,7 +3226,7 @@
         <v>127</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>85</v>
+        <v>295</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>85</v>
@@ -3144,8 +3237,11 @@
       <c r="L19" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>225</v>
       </c>
@@ -3171,7 +3267,7 @@
         <v>127</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>100</v>
+        <v>296</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>100</v>
@@ -3182,8 +3278,11 @@
       <c r="L20" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>226</v>
       </c>
@@ -3209,7 +3308,7 @@
         <v>127</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>100</v>
+        <v>297</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>100</v>
@@ -3220,8 +3319,11 @@
       <c r="L21" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>227</v>
       </c>
@@ -3247,7 +3349,7 @@
         <v>127</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>100</v>
+        <v>298</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>100</v>
@@ -3258,8 +3360,11 @@
       <c r="L22" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>228</v>
       </c>
@@ -3285,7 +3390,7 @@
         <v>127</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>100</v>
+        <v>299</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>100</v>
@@ -3296,8 +3401,11 @@
       <c r="L23" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>229</v>
       </c>
@@ -3323,7 +3431,7 @@
         <v>127</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>100</v>
+        <v>300</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>100</v>
@@ -3334,8 +3442,11 @@
       <c r="L24" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>230</v>
       </c>
@@ -3361,7 +3472,7 @@
         <v>127</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>100</v>
+        <v>301</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>100</v>
@@ -3372,8 +3483,11 @@
       <c r="L25" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>231</v>
       </c>
@@ -3399,7 +3513,7 @@
         <v>127</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>100</v>
+        <v>302</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>100</v>
@@ -3410,8 +3524,11 @@
       <c r="L26" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>232</v>
       </c>
@@ -3437,7 +3554,7 @@
         <v>127</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>100</v>
+        <v>303</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>100</v>
@@ -3448,8 +3565,11 @@
       <c r="L27" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>233</v>
       </c>
@@ -3475,7 +3595,7 @@
         <v>127</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>100</v>
+        <v>304</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>100</v>
@@ -3486,8 +3606,11 @@
       <c r="L28" s="1" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>234</v>
       </c>
@@ -3513,7 +3636,7 @@
         <v>127</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>100</v>
+        <v>305</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>100</v>
@@ -3524,8 +3647,12 @@
       <c r="L29" s="1" t="s">
         <v>100</v>
       </c>
+      <c r="M29" s="1" t="s">
+        <v>100</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -3536,7 +3663,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4702,7 +4829,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4721,81 +4848,29 @@
         <v>274</v>
       </c>
       <c r="C1" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="D1" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="B2" t="s">
-        <v>275</v>
-      </c>
-      <c r="C2" t="s">
-        <v>286</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>291</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="B3" t="s">
-        <v>277</v>
-      </c>
-      <c r="C3" t="s">
-        <v>288</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>177</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="D3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="B4" t="s">
-        <v>276</v>
-      </c>
-      <c r="C4" t="s">
-        <v>287</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>176</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="B5" t="s">
-        <v>278</v>
-      </c>
-      <c r="C5" t="s">
-        <v>289</v>
-      </c>
-      <c r="D5" t="s">
-        <v>178</v>
-      </c>
+      <c r="A5" s="1"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>284</v>
-      </c>
-      <c r="B6" t="s">
-        <v>279</v>
-      </c>
-      <c r="C6" t="s">
-        <v>290</v>
-      </c>
-      <c r="D6" t="s">
-        <v>179</v>
-      </c>
+      <c r="A6" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Abstraction Utilize for ID Generator - DEVELOP
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
+++ b/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olaf\IdeaProjects\OODJ\src\main\resources\Data\SampleDataXlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanh\IdeaProjects\G5-2402-OODJ\src\main\resources\Data\SampleDataXlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02382B9-25BC-4408-A4EA-F56178C959DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FBDFD9-7902-40F3-89E7-E7A49CB972BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11730" yWindow="2715" windowWidth="22095" windowHeight="17550" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6525" yWindow="990" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="310">
   <si>
     <t>id</t>
   </si>
@@ -558,397 +558,409 @@
     <t>39904006</t>
   </si>
   <si>
+    <t>INVESTIGATION</t>
+  </si>
+  <si>
+    <t>FINAL_YEAR</t>
+  </si>
+  <si>
+    <t>CAPSTONE_1</t>
+  </si>
+  <si>
+    <t>CAPSTONE_2</t>
+  </si>
+  <si>
+    <t>51119855</t>
+  </si>
+  <si>
+    <t>51074390</t>
+  </si>
+  <si>
+    <t>16998057</t>
+  </si>
+  <si>
+    <t>83642670</t>
+  </si>
+  <si>
+    <t>78229912</t>
+  </si>
+  <si>
+    <t>88608036</t>
+  </si>
+  <si>
+    <t>31957573</t>
+  </si>
+  <si>
+    <t>95518749</t>
+  </si>
+  <si>
+    <t>81080865</t>
+  </si>
+  <si>
+    <t>75508701</t>
+  </si>
+  <si>
+    <t>59262392</t>
+  </si>
+  <si>
+    <t>72921720</t>
+  </si>
+  <si>
+    <t>55020419</t>
+  </si>
+  <si>
+    <t>98130811</t>
+  </si>
+  <si>
+    <t>Swift</t>
+  </si>
+  <si>
+    <t>88722038</t>
+  </si>
+  <si>
+    <t>97288953</t>
+  </si>
+  <si>
+    <t>36887009</t>
+  </si>
+  <si>
+    <t>90776138</t>
+  </si>
+  <si>
+    <t>39596939</t>
+  </si>
+  <si>
+    <t>37346231</t>
+  </si>
+  <si>
+    <t>42151499</t>
+  </si>
+  <si>
+    <t>54981796</t>
+  </si>
+  <si>
+    <t>31492867</t>
+  </si>
+  <si>
+    <t>73889408</t>
+  </si>
+  <si>
+    <t>16335098</t>
+  </si>
+  <si>
+    <t>16172465</t>
+  </si>
+  <si>
+    <t>2127241</t>
+  </si>
+  <si>
+    <t>63621304</t>
+  </si>
+  <si>
+    <t>28548294</t>
+  </si>
+  <si>
+    <t>42258355</t>
+  </si>
+  <si>
+    <t>82975243</t>
+  </si>
+  <si>
+    <t>77629561</t>
+  </si>
+  <si>
+    <t>66882174</t>
+  </si>
+  <si>
+    <t>67351802</t>
+  </si>
+  <si>
+    <t>44467240</t>
+  </si>
+  <si>
+    <t>98294670</t>
+  </si>
+  <si>
+    <t>44766076</t>
+  </si>
+  <si>
+    <t>16048967</t>
+  </si>
+  <si>
+    <t>59626184</t>
+  </si>
+  <si>
+    <t>6036554</t>
+  </si>
+  <si>
+    <t>24668260</t>
+  </si>
+  <si>
+    <t>77416905</t>
+  </si>
+  <si>
+    <t>32857478</t>
+  </si>
+  <si>
+    <t>89608676</t>
+  </si>
+  <si>
+    <t>88870563</t>
+  </si>
+  <si>
+    <t>43454090</t>
+  </si>
+  <si>
+    <t>31159280</t>
+  </si>
+  <si>
+    <t>24492695</t>
+  </si>
+  <si>
+    <t>86195582</t>
+  </si>
+  <si>
+    <t>53997265</t>
+  </si>
+  <si>
+    <t>84245467</t>
+  </si>
+  <si>
+    <t>53668659</t>
+  </si>
+  <si>
+    <t>20230431</t>
+  </si>
+  <si>
+    <t>69967900</t>
+  </si>
+  <si>
+    <t>marked_at</t>
+  </si>
+  <si>
+    <t>3268572</t>
+  </si>
+  <si>
+    <t>2022-04-09 00:00:00</t>
+  </si>
+  <si>
+    <t>2026-01-01</t>
+  </si>
+  <si>
+    <t>2024-08-01</t>
+  </si>
+  <si>
+    <t>PENDING_CONFIRM</t>
+  </si>
+  <si>
+    <t>2024-01-01 00:00:00</t>
+  </si>
+  <si>
+    <t>REJECTED</t>
+  </si>
+  <si>
+    <t>MARKED</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>80</t>
+  </si>
+  <si>
+    <t>81</t>
+  </si>
+  <si>
+    <t>82</t>
+  </si>
+  <si>
+    <t>83</t>
+  </si>
+  <si>
+    <t>84</t>
+  </si>
+  <si>
+    <t>85</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>88</t>
+  </si>
+  <si>
+    <t>89</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>91</t>
+  </si>
+  <si>
+    <t>92</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>94</t>
+  </si>
+  <si>
+    <t>95</t>
+  </si>
+  <si>
+    <t>96</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>103</t>
+  </si>
+  <si>
+    <t>104</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>106</t>
+  </si>
+  <si>
+    <t>BOOKED</t>
+  </si>
+  <si>
+    <t>OVERDUE</t>
+  </si>
+  <si>
+    <t>2024-08-01 00:00:00</t>
+  </si>
+  <si>
+    <t>reportName</t>
+  </si>
+  <si>
+    <t>reportPath</t>
+  </si>
+  <si>
+    <t>REPORT</t>
+  </si>
+  <si>
+    <t>comment</t>
+  </si>
+  <si>
+    <t>comment1</t>
+  </si>
+  <si>
+    <t>comment2</t>
+  </si>
+  <si>
+    <t>comment3</t>
+  </si>
+  <si>
+    <t>comment4</t>
+  </si>
+  <si>
+    <t>comment5</t>
+  </si>
+  <si>
+    <t>comment6</t>
+  </si>
+  <si>
+    <t>comment7</t>
+  </si>
+  <si>
+    <t>comment8</t>
+  </si>
+  <si>
+    <t>comment9</t>
+  </si>
+  <si>
+    <t>comment10</t>
+  </si>
+  <si>
+    <t>comment11</t>
+  </si>
+  <si>
+    <t>comment12</t>
+  </si>
+  <si>
+    <t>comment13</t>
+  </si>
+  <si>
+    <t>comment14</t>
+  </si>
+  <si>
+    <t>comment15</t>
+  </si>
+  <si>
+    <t>comment16</t>
+  </si>
+  <si>
+    <t>comment17</t>
+  </si>
+  <si>
+    <t>comment18</t>
+  </si>
+  <si>
+    <t>comment19</t>
+  </si>
+  <si>
+    <t>comment20</t>
+  </si>
+  <si>
+    <t>comment21</t>
+  </si>
+  <si>
+    <t>comment22</t>
+  </si>
+  <si>
+    <t>comment23</t>
+  </si>
+  <si>
+    <t>comment24</t>
+  </si>
+  <si>
+    <t>comment25</t>
+  </si>
+  <si>
+    <t>comment26</t>
+  </si>
+  <si>
+    <t>comment27</t>
+  </si>
+  <si>
+    <t>comment28</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>src/main/resources/Data/SampleDataXlsx/FinalYearProject.pdf</t>
+  </si>
+  <si>
     <t>PENDING_SUBMIT</t>
   </si>
   <si>
-    <t>INVESTIGATION</t>
-  </si>
-  <si>
-    <t>FINAL_YEAR</t>
-  </si>
-  <si>
-    <t>CAPSTONE_1</t>
-  </si>
-  <si>
-    <t>CAPSTONE_2</t>
-  </si>
-  <si>
-    <t>51119855</t>
-  </si>
-  <si>
-    <t>51074390</t>
-  </si>
-  <si>
-    <t>16998057</t>
-  </si>
-  <si>
-    <t>83642670</t>
-  </si>
-  <si>
-    <t>78229912</t>
-  </si>
-  <si>
-    <t>88608036</t>
-  </si>
-  <si>
-    <t>31957573</t>
-  </si>
-  <si>
-    <t>95518749</t>
-  </si>
-  <si>
-    <t>81080865</t>
-  </si>
-  <si>
-    <t>75508701</t>
-  </si>
-  <si>
-    <t>59262392</t>
-  </si>
-  <si>
-    <t>72921720</t>
-  </si>
-  <si>
-    <t>55020419</t>
-  </si>
-  <si>
-    <t>98130811</t>
-  </si>
-  <si>
-    <t>Swift</t>
-  </si>
-  <si>
-    <t>88722038</t>
-  </si>
-  <si>
-    <t>97288953</t>
-  </si>
-  <si>
-    <t>36887009</t>
-  </si>
-  <si>
-    <t>90776138</t>
-  </si>
-  <si>
-    <t>39596939</t>
-  </si>
-  <si>
-    <t>37346231</t>
-  </si>
-  <si>
-    <t>42151499</t>
-  </si>
-  <si>
-    <t>54981796</t>
-  </si>
-  <si>
-    <t>31492867</t>
-  </si>
-  <si>
-    <t>73889408</t>
-  </si>
-  <si>
-    <t>16335098</t>
-  </si>
-  <si>
-    <t>16172465</t>
-  </si>
-  <si>
-    <t>2127241</t>
-  </si>
-  <si>
-    <t>63621304</t>
-  </si>
-  <si>
-    <t>28548294</t>
-  </si>
-  <si>
-    <t>42258355</t>
-  </si>
-  <si>
-    <t>82975243</t>
-  </si>
-  <si>
-    <t>77629561</t>
-  </si>
-  <si>
-    <t>66882174</t>
-  </si>
-  <si>
-    <t>67351802</t>
-  </si>
-  <si>
-    <t>44467240</t>
-  </si>
-  <si>
-    <t>98294670</t>
-  </si>
-  <si>
-    <t>44766076</t>
-  </si>
-  <si>
-    <t>16048967</t>
-  </si>
-  <si>
-    <t>59626184</t>
-  </si>
-  <si>
-    <t>6036554</t>
-  </si>
-  <si>
-    <t>24668260</t>
-  </si>
-  <si>
-    <t>77416905</t>
-  </si>
-  <si>
-    <t>32857478</t>
-  </si>
-  <si>
-    <t>89608676</t>
-  </si>
-  <si>
-    <t>88870563</t>
-  </si>
-  <si>
-    <t>43454090</t>
-  </si>
-  <si>
-    <t>31159280</t>
-  </si>
-  <si>
-    <t>24492695</t>
-  </si>
-  <si>
-    <t>86195582</t>
-  </si>
-  <si>
-    <t>53997265</t>
-  </si>
-  <si>
-    <t>84245467</t>
-  </si>
-  <si>
-    <t>53668659</t>
-  </si>
-  <si>
-    <t>20230431</t>
-  </si>
-  <si>
-    <t>69967900</t>
-  </si>
-  <si>
-    <t>marked_at</t>
-  </si>
-  <si>
-    <t>3268572</t>
-  </si>
-  <si>
-    <t>2022-04-09 00:00:00</t>
-  </si>
-  <si>
-    <t>2026-01-01</t>
-  </si>
-  <si>
-    <t>2024-08-01</t>
-  </si>
-  <si>
-    <t>PENDING_CONFIRM</t>
-  </si>
-  <si>
-    <t>2024-01-01 00:00:00</t>
-  </si>
-  <si>
-    <t>REJECTED</t>
-  </si>
-  <si>
-    <t>MARKED</t>
-  </si>
-  <si>
-    <t>99</t>
-  </si>
-  <si>
-    <t>80</t>
-  </si>
-  <si>
-    <t>81</t>
-  </si>
-  <si>
-    <t>82</t>
-  </si>
-  <si>
-    <t>83</t>
-  </si>
-  <si>
-    <t>84</t>
-  </si>
-  <si>
-    <t>85</t>
-  </si>
-  <si>
-    <t>86</t>
-  </si>
-  <si>
-    <t>87</t>
-  </si>
-  <si>
-    <t>88</t>
-  </si>
-  <si>
-    <t>89</t>
-  </si>
-  <si>
-    <t>90</t>
-  </si>
-  <si>
-    <t>91</t>
-  </si>
-  <si>
-    <t>92</t>
-  </si>
-  <si>
-    <t>93</t>
-  </si>
-  <si>
-    <t>94</t>
-  </si>
-  <si>
-    <t>95</t>
-  </si>
-  <si>
-    <t>96</t>
-  </si>
-  <si>
-    <t>97</t>
-  </si>
-  <si>
-    <t>98</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>101</t>
-  </si>
-  <si>
-    <t>102</t>
-  </si>
-  <si>
-    <t>103</t>
-  </si>
-  <si>
-    <t>104</t>
-  </si>
-  <si>
-    <t>105</t>
-  </si>
-  <si>
-    <t>106</t>
-  </si>
-  <si>
-    <t>BOOKED</t>
-  </si>
-  <si>
-    <t>OVERDUE</t>
-  </si>
-  <si>
-    <t>2024-08-01 00:00:00</t>
-  </si>
-  <si>
-    <t>reportName</t>
-  </si>
-  <si>
-    <t>reportPath</t>
-  </si>
-  <si>
-    <t>REPORT</t>
-  </si>
-  <si>
-    <t>comment</t>
-  </si>
-  <si>
-    <t>comment1</t>
-  </si>
-  <si>
-    <t>comment2</t>
-  </si>
-  <si>
-    <t>comment3</t>
-  </si>
-  <si>
-    <t>comment4</t>
-  </si>
-  <si>
-    <t>comment5</t>
-  </si>
-  <si>
-    <t>comment6</t>
-  </si>
-  <si>
-    <t>comment7</t>
-  </si>
-  <si>
-    <t>comment8</t>
-  </si>
-  <si>
-    <t>comment9</t>
-  </si>
-  <si>
-    <t>comment10</t>
-  </si>
-  <si>
-    <t>comment11</t>
-  </si>
-  <si>
-    <t>comment12</t>
-  </si>
-  <si>
-    <t>comment13</t>
-  </si>
-  <si>
-    <t>comment14</t>
-  </si>
-  <si>
-    <t>comment15</t>
-  </si>
-  <si>
-    <t>comment16</t>
-  </si>
-  <si>
-    <t>comment17</t>
-  </si>
-  <si>
-    <t>comment18</t>
-  </si>
-  <si>
-    <t>comment19</t>
-  </si>
-  <si>
-    <t>comment20</t>
-  </si>
-  <si>
-    <t>comment21</t>
-  </si>
-  <si>
-    <t>comment22</t>
-  </si>
-  <si>
-    <t>comment23</t>
-  </si>
-  <si>
-    <t>comment24</t>
-  </si>
-  <si>
-    <t>comment25</t>
-  </si>
-  <si>
-    <t>comment26</t>
-  </si>
-  <si>
-    <t>comment27</t>
-  </si>
-  <si>
-    <t>comment28</t>
+    <t>MARKED_2</t>
   </si>
 </sst>
 </file>
@@ -1369,7 +1381,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>15</v>
@@ -1439,7 +1451,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
@@ -1474,7 +1486,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>9</v>
@@ -1509,7 +1521,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>8</v>
@@ -1544,7 +1556,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>21</v>
@@ -1579,7 +1591,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>23</v>
@@ -1614,7 +1626,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>25</v>
@@ -1649,7 +1661,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>41</v>
@@ -1684,7 +1696,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>43</v>
@@ -1719,7 +1731,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>45</v>
@@ -1754,7 +1766,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>46</v>
@@ -1789,7 +1801,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>47</v>
@@ -1824,7 +1836,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>44</v>
@@ -1859,7 +1871,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>48</v>
@@ -1900,7 +1912,7 @@
         <v>60</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>59</v>
@@ -1977,7 +1989,7 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>91</v>
@@ -1989,7 +2001,7 @@
         <v>97</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>100</v>
@@ -2000,7 +2012,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>93</v>
@@ -2035,7 +2047,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2084,10 +2096,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>106</v>
@@ -2096,16 +2108,16 @@
         <v>174</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>85</v>
@@ -2119,25 +2131,25 @@
         <v>101</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>107</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>85</v>
@@ -2148,28 +2160,28 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>108</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>85</v>
@@ -2180,28 +2192,28 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>109</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>85</v>
@@ -2212,28 +2224,28 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>110</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>85</v>
@@ -2244,10 +2256,10 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>111</v>
@@ -2256,16 +2268,16 @@
         <v>174</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>97</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>85</v>
@@ -2276,22 +2288,22 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>112</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>96</v>
@@ -2308,22 +2320,22 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>113</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>96</v>
@@ -2340,22 +2352,22 @@
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>114</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>96</v>
@@ -2372,22 +2384,22 @@
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>115</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>96</v>
@@ -2404,10 +2416,10 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>116</v>
@@ -2416,10 +2428,10 @@
         <v>174</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>96</v>
@@ -2446,7 +2458,7 @@
   <dimension ref="A1:M29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2488,13 +2500,13 @@
         <v>172</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>173</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>4</v>
@@ -2505,31 +2517,31 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>127</v>
+        <v>305</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>272</v>
+        <v>309</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>85</v>
@@ -2546,31 +2558,31 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>85</v>
@@ -2587,31 +2599,31 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="H4" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>85</v>
@@ -2628,7 +2640,7 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>127</v>
@@ -2637,22 +2649,22 @@
         <v>101</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>85</v>
@@ -2669,7 +2681,7 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>127</v>
@@ -2678,22 +2690,22 @@
         <v>101</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>85</v>
@@ -2710,7 +2722,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>127</v>
@@ -2719,22 +2731,22 @@
         <v>101</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>85</v>
@@ -2751,31 +2763,31 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>85</v>
@@ -2792,31 +2804,31 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F9" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="H9" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>85</v>
@@ -2833,31 +2845,31 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F10" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G10" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="H10" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>85</v>
@@ -2874,31 +2886,31 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>85</v>
@@ -2915,31 +2927,31 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>85</v>
@@ -2956,31 +2968,31 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>85</v>
@@ -2997,31 +3009,31 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>85</v>
@@ -3038,31 +3050,31 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F15" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="H15" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>85</v>
@@ -3079,31 +3091,31 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F16" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>176</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>85</v>
@@ -3120,31 +3132,31 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>127</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>85</v>
@@ -3161,31 +3173,31 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>127</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>85</v>
@@ -3202,31 +3214,31 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>127</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>85</v>
@@ -3243,31 +3255,31 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>127</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>100</v>
@@ -3284,31 +3296,31 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>127</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>100</v>
@@ -3325,31 +3337,31 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>127</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>100</v>
@@ -3366,31 +3378,31 @@
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>127</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>100</v>
@@ -3407,31 +3419,31 @@
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>127</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>100</v>
@@ -3448,31 +3460,31 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>127</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>100</v>
@@ -3489,31 +3501,31 @@
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>127</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>100</v>
@@ -3530,31 +3542,31 @@
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>127</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>100</v>
@@ -3571,31 +3583,31 @@
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>127</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>100</v>
@@ -3612,31 +3624,31 @@
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>127</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>175</v>
+        <v>308</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>127</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>100</v>
@@ -3719,25 +3731,25 @@
         <v>146</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>85</v>
@@ -3751,25 +3763,25 @@
         <v>147</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>85</v>
@@ -3783,25 +3795,25 @@
         <v>148</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>85</v>
@@ -3818,22 +3830,22 @@
         <v>101</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>85</v>
@@ -3850,22 +3862,22 @@
         <v>101</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>85</v>
@@ -3882,22 +3894,22 @@
         <v>101</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>85</v>
@@ -3911,25 +3923,25 @@
         <v>152</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F8" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>242</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>85</v>
@@ -3943,25 +3955,25 @@
         <v>153</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>85</v>
@@ -3975,25 +3987,25 @@
         <v>154</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>85</v>
@@ -4007,25 +4019,25 @@
         <v>138</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>85</v>
@@ -4039,25 +4051,25 @@
         <v>139</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>85</v>
@@ -4071,25 +4083,25 @@
         <v>140</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>85</v>
@@ -4103,25 +4115,25 @@
         <v>141</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="D14" s="1" t="s">
-        <v>190</v>
-      </c>
       <c r="E14" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>85</v>
@@ -4135,25 +4147,25 @@
         <v>142</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>85</v>
@@ -4167,25 +4179,25 @@
         <v>143</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>85</v>
@@ -4199,25 +4211,25 @@
         <v>144</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>85</v>
@@ -4231,25 +4243,25 @@
         <v>145</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>85</v>
@@ -4263,25 +4275,25 @@
         <v>155</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>158</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>100</v>
@@ -4295,16 +4307,16 @@
         <v>156</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>100</v>
@@ -4313,7 +4325,7 @@
         <v>158</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>100</v>
@@ -4327,16 +4339,16 @@
         <v>157</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>100</v>
@@ -4345,7 +4357,7 @@
         <v>158</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>100</v>
@@ -4359,16 +4371,16 @@
         <v>159</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>100</v>
@@ -4377,7 +4389,7 @@
         <v>158</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>100</v>
@@ -4391,16 +4403,16 @@
         <v>160</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>100</v>
@@ -4409,7 +4421,7 @@
         <v>158</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>100</v>
@@ -4423,16 +4435,16 @@
         <v>161</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>100</v>
@@ -4441,7 +4453,7 @@
         <v>158</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>100</v>
@@ -4455,25 +4467,25 @@
         <v>162</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>100</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>100</v>
@@ -4487,25 +4499,25 @@
         <v>163</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>100</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>100</v>
@@ -4519,25 +4531,25 @@
         <v>164</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>100</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>100</v>
@@ -4551,25 +4563,25 @@
         <v>165</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>100</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>100</v>
@@ -4583,25 +4595,25 @@
         <v>166</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>94</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>100</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>100</v>
@@ -4659,10 +4671,10 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>127</v>
@@ -4685,7 +4697,7 @@
         <v>121</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>127</v>
@@ -4708,7 +4720,7 @@
         <v>122</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>127</v>
@@ -4731,7 +4743,7 @@
         <v>118</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>127</v>
@@ -4754,7 +4766,7 @@
         <v>119</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>127</v>
@@ -4777,7 +4789,7 @@
         <v>120</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>127</v>
@@ -4800,7 +4812,7 @@
         <v>121</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>127</v>
@@ -4829,7 +4841,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="G17" activeCellId="1" sqref="C8 G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4845,18 +4857,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C1" t="s">
         <v>274</v>
-      </c>
-      <c r="C1" t="s">
-        <v>275</v>
       </c>
       <c r="D1" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="B2" t="s">
+        <v>306</v>
+      </c>
+      <c r="C2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>

</xml_diff>

<commit_message>
Fix error - Module Table
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
+++ b/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olaf\IdeaProjects\OODJ\src\main\resources\Data\SampleDataXlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b8e73236fe8d0ac8/Documents/GitHub/G5-2402-OODJ/src/main/resources/Data/SampleDataXlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02382B9-25BC-4408-A4EA-F56178C959DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{E02382B9-25BC-4408-A4EA-F56178C959DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56C7F360-17A8-4939-9CB0-91D7C24ADB0C}"/>
   <bookViews>
-    <workbookView xWindow="11730" yWindow="2715" windowWidth="22095" windowHeight="17550" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11295" firstSheet="2" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1066" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="309">
   <si>
     <t>id</t>
   </si>
@@ -949,6 +949,15 @@
   </si>
   <si>
     <t>comment28</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -2035,7 +2044,7 @@
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2445,7 +2454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBCA89A-312D-41B5-8992-19B0B67944A1}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
@@ -4828,8 +4837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4C6E3A0-FE14-4583-BA4F-E8188E3B166D}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4855,8 +4864,18 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="D2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" t="s">
+        <v>307</v>
+      </c>
+      <c r="C2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>

</xml_diff>

<commit_message>
Fix bugs - ManagerViewReport
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
+++ b/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chanh\IdeaProjects\G5-2402-OODJ\src\main\resources\Data\SampleDataXlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b8e73236fe8d0ac8/Documents/GitHub/G5-2402-OODJ/src/main/resources/Data/SampleDataXlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28FBDFD9-7902-40F3-89E7-E7A49CB972BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{28FBDFD9-7902-40F3-89E7-E7A49CB972BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8FC00FA-5B09-48B2-A055-8B87020E224B}"/>
   <bookViews>
-    <workbookView xWindow="6525" yWindow="990" windowWidth="21600" windowHeight="11295" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1071" uniqueCount="310">
   <si>
     <t>id</t>
   </si>
@@ -858,9 +858,6 @@
     <t>reportPath</t>
   </si>
   <si>
-    <t>REPORT</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -961,6 +958,9 @@
   </si>
   <si>
     <t>MARKED_2</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -1023,6 +1023,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1291,10 +1295,10 @@
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
     <col min="2" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -1954,7 +1958,7 @@
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" bestFit="1" customWidth="1"/>
@@ -2044,13 +2048,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9D51FCF-93DA-4829-9D15-DA3415652AC5}">
-  <dimension ref="A1:J12"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.42578125" style="1" bestFit="1" customWidth="1"/>
@@ -2446,6 +2450,12 @@
         <v>100</v>
       </c>
     </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2457,11 +2467,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBCA89A-312D-41B5-8992-19B0B67944A1}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -2494,13 +2502,13 @@
         <v>170</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>171</v>
+        <v>309</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>172</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>173</v>
@@ -2520,7 +2528,7 @@
         <v>206</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>196</v>
@@ -2532,16 +2540,16 @@
         <v>272</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>275</v>
+        <v>175</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>254</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>85</v>
@@ -2573,7 +2581,7 @@
         <v>272</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>175</v>
@@ -2582,7 +2590,7 @@
         <v>254</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>85</v>
@@ -2614,7 +2622,7 @@
         <v>272</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>175</v>
@@ -2623,7 +2631,7 @@
         <v>254</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>85</v>
@@ -2655,7 +2663,7 @@
         <v>272</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>176</v>
@@ -2664,7 +2672,7 @@
         <v>254</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>85</v>
@@ -2696,7 +2704,7 @@
         <v>272</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>176</v>
@@ -2705,7 +2713,7 @@
         <v>254</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>85</v>
@@ -2737,7 +2745,7 @@
         <v>272</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>176</v>
@@ -2746,7 +2754,7 @@
         <v>254</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J7" s="1" t="s">
         <v>85</v>
@@ -2778,7 +2786,7 @@
         <v>272</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>175</v>
@@ -2787,7 +2795,7 @@
         <v>254</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>85</v>
@@ -2819,7 +2827,7 @@
         <v>272</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>175</v>
@@ -2828,7 +2836,7 @@
         <v>254</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>85</v>
@@ -2860,7 +2868,7 @@
         <v>272</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>175</v>
@@ -2869,7 +2877,7 @@
         <v>254</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>85</v>
@@ -2901,7 +2909,7 @@
         <v>272</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>177</v>
@@ -2910,7 +2918,7 @@
         <v>254</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>85</v>
@@ -2942,7 +2950,7 @@
         <v>272</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>176</v>
@@ -2951,7 +2959,7 @@
         <v>254</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>85</v>
@@ -2983,7 +2991,7 @@
         <v>272</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>176</v>
@@ -2992,7 +3000,7 @@
         <v>254</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>85</v>
@@ -3024,7 +3032,7 @@
         <v>272</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>178</v>
@@ -3033,7 +3041,7 @@
         <v>254</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>85</v>
@@ -3065,7 +3073,7 @@
         <v>272</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>175</v>
@@ -3074,7 +3082,7 @@
         <v>254</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>85</v>
@@ -3106,7 +3114,7 @@
         <v>272</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>175</v>
@@ -3115,7 +3123,7 @@
         <v>254</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>85</v>
@@ -3147,7 +3155,7 @@
         <v>272</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>176</v>
@@ -3156,7 +3164,7 @@
         <v>127</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>85</v>
@@ -3188,7 +3196,7 @@
         <v>272</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>176</v>
@@ -3197,7 +3205,7 @@
         <v>127</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>85</v>
@@ -3229,7 +3237,7 @@
         <v>272</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G19" s="1" t="s">
         <v>176</v>
@@ -3238,7 +3246,7 @@
         <v>127</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>85</v>
@@ -3270,7 +3278,7 @@
         <v>236</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G20" s="1" t="s">
         <v>177</v>
@@ -3279,7 +3287,7 @@
         <v>127</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>100</v>
@@ -3311,7 +3319,7 @@
         <v>236</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>177</v>
@@ -3320,7 +3328,7 @@
         <v>127</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>100</v>
@@ -3352,7 +3360,7 @@
         <v>236</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>176</v>
@@ -3361,7 +3369,7 @@
         <v>127</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>100</v>
@@ -3393,7 +3401,7 @@
         <v>236</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>176</v>
@@ -3402,7 +3410,7 @@
         <v>127</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>100</v>
@@ -3434,7 +3442,7 @@
         <v>236</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G24" s="1" t="s">
         <v>176</v>
@@ -3443,7 +3451,7 @@
         <v>127</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>100</v>
@@ -3475,7 +3483,7 @@
         <v>236</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>176</v>
@@ -3484,7 +3492,7 @@
         <v>127</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>100</v>
@@ -3516,7 +3524,7 @@
         <v>236</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G26" s="1" t="s">
         <v>176</v>
@@ -3525,7 +3533,7 @@
         <v>127</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>100</v>
@@ -3557,7 +3565,7 @@
         <v>236</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>176</v>
@@ -3566,7 +3574,7 @@
         <v>127</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>100</v>
@@ -3598,7 +3606,7 @@
         <v>236</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>178</v>
@@ -3607,7 +3615,7 @@
         <v>127</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>100</v>
@@ -3639,7 +3647,7 @@
         <v>236</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G29" s="1" t="s">
         <v>178</v>
@@ -3648,7 +3656,7 @@
         <v>127</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>100</v>
@@ -3678,7 +3686,7 @@
       <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -4635,7 +4643,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
@@ -4868,13 +4876,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="B2" t="s">
         <v>305</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>306</v>
-      </c>
-      <c r="C2" t="s">
-        <v>307</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>176</v>

</xml_diff>

<commit_message>
Test Environment Setup with data - UPDATE
</commit_message>
<xml_diff>
--- a/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
+++ b/src/main/resources/Data/SampleDataXlsx/G5_OODJ_Sample_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olaf\IdeaProjects\OODJ\G5-2402-OODJ\src\main\resources\Data\SampleDataXlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99B0ADD-5D40-44CA-B62B-0FCF61F32D84}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DEF151-5929-4547-BCFF-A843234D382A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11910" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User" sheetId="1" r:id="rId1"/>
@@ -1278,8 +1278,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2035,7 +2035,7 @@
   <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2449,8 +2449,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBCA89A-312D-41B5-8992-19B0B67944A1}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3667,7 +3667,7 @@
   <dimension ref="A1:J29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N23" sqref="N23"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>